<commit_message>
Updates before I leave.
</commit_message>
<xml_diff>
--- a/RESULTS/NNTestResults-1Layer-4To256Nodes-32Epochs.xlsx
+++ b/RESULTS/NNTestResults-1Layer-4To256Nodes-32Epochs.xlsx
@@ -139,37 +139,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2093,13 +2063,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576 E1:G1">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="PCLOUD">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="PCLOUD">
       <formula>NOT(ISERROR(SEARCH("PCLOUD",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="IDEPTH">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="IDEPTH">
       <formula>NOT(ISERROR(SEARCH("IDEPTH",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="ICOLOR">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="ICOLOR">
       <formula>NOT(ISERROR(SEARCH("ICOLOR",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2112,7 +2082,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="F17" sqref="A17:F17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3022,24 +2992,24 @@
     <sortCondition ref="B2:B37"/>
   </sortState>
   <conditionalFormatting sqref="D1:D22 E1:F1">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="PCLOUD">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="PCLOUD">
       <formula>NOT(ISERROR(SEARCH("PCLOUD",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="IDEPTH">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="IDEPTH">
       <formula>NOT(ISERROR(SEARCH("IDEPTH",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="ICOLOR">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="ICOLOR">
       <formula>NOT(ISERROR(SEARCH("ICOLOR",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D37">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="PCLOUD">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="PCLOUD">
       <formula>NOT(ISERROR(SEARCH("PCLOUD",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="IDEPTH">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="IDEPTH">
       <formula>NOT(ISERROR(SEARCH("IDEPTH",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="ICOLOR">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="ICOLOR">
       <formula>NOT(ISERROR(SEARCH("ICOLOR",D23)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>